<commit_message>
Merge main into current branch
</commit_message>
<xml_diff>
--- a/apps/anthro/static/template_en.xlsx
+++ b/apps/anthro/static/template_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felhasználó\PycharmProjects\PythonProject1\anthro-web\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felhasználó\PycharmProjects\PythonProject1\monorepo\apps\anthro\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4013522-6615-4F83-A4BB-98E3C81BC22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D2CAF1-9E26-4C67-B19F-72A317E31CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FD0E5E17-5FD6-4C4E-83A4-EA2AA6AF8D9F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>TR</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Sitting height</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Team</t>
   </si>
 </sst>
 </file>
@@ -520,123 +526,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B99430F-2D99-4445-B3BE-ECA3C8ECB2A2}">
-  <dimension ref="A1:AF33"/>
+  <dimension ref="A1:AH33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="14" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="32" width="8.7265625" style="5"/>
+    <col min="5" max="5" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="34" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AB1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AD1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AF1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
-      <c r="B2" s="1"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+    <row r="2" spans="1:34">
+      <c r="D2" s="1"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -663,14 +673,16 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
-    </row>
-    <row r="3" spans="1:32">
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+    </row>
+    <row r="3" spans="1:34">
       <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -697,14 +709,16 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
-    </row>
-    <row r="4" spans="1:32">
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34">
       <c r="A4" s="4"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -731,14 +745,16 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+    </row>
+    <row r="5" spans="1:34">
       <c r="A5" s="4"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -765,90 +781,92 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
-    </row>
-    <row r="6" spans="1:32">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:32">
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:32">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:32">
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:32">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:32">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:32">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:32">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:32">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:32">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:32">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:2">
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="2:2">
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="3"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:34">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:34">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:34">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:34">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:34">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:34">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:34">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:34">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="4:4">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="4:4">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="4:4">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="4:4">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="4:4">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="4:4">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="4:4">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="4:4">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="4:4">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="4:4">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="4:4">
+      <c r="D33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>